<commit_message>
Add `task-10` in `game-theory`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/game-theory/Бронников Егор ПМ-1901 - Задача линейного программирование.xlsx
+++ b/3-course-6-semester/game-theory/Бронников Егор ПМ-1901 - Задача линейного программирование.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Documents\github\university\3-course-6-semester\game-theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2110B-6C92-483E-9992-F34EED208B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AD8CC9-3F70-4075-B5AA-FD74A2EE12C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{090A3530-518D-493E-A9AB-B02315E3DE31}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Обычная матрица'!$C$5:$G$5,'Обычная матрица'!$I$10</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Преобразованная матрица'!$L$21:$M$24,'Преобразованная матрица'!$M$25</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Преобразованная матрица'!$G$20:$K$20</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
@@ -30,7 +30,7 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Обычная матрица'!$H$6:$H$9</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Преобразованная матрица'!$G$25:$K$25</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Преобразованная матрица'!$L$21:$L$24</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Обычная матрица'!$I$4</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Преобразованная матрица'!$G$25:$K$25</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
@@ -184,13 +184,17 @@
     <t>delta</t>
   </si>
   <si>
-    <t>Целевая функция</t>
+    <t>1/V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -567,7 +571,105 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -580,7 +682,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -593,34 +708,60 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -635,33 +776,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -671,55 +786,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -729,23 +799,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -753,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -814,7 +871,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,100 +880,119 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1272,31 +1347,31 @@
       <c r="H4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="34">
         <f>SUM(C5:G5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <v>0</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="30">
         <v>0.19039780521262004</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="30">
         <v>0.19149519890260638</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="30">
         <v>0.31522633744855977</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="30">
         <v>0.30288065843621387</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="55"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -1320,11 +1395,11 @@
       <c r="G6" s="3">
         <v>4</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="35">
         <f>SUMPRODUCT($C$5:$G$5,C6:G6)</f>
         <v>2.3423868312757206</v>
       </c>
-      <c r="I6" s="55"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -1348,11 +1423,11 @@
       <c r="G7" s="6">
         <v>8</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="35">
         <f t="shared" ref="H7:H9" si="0">SUMPRODUCT($C$5:$G$5,C7:G7)</f>
         <v>2.3423868312757188</v>
       </c>
-      <c r="I7" s="55"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -1376,11 +1451,11 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="35">
         <f t="shared" si="0"/>
         <v>2.3423868312757206</v>
       </c>
-      <c r="I8" s="55"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -1404,17 +1479,17 @@
       <c r="G9" s="6">
         <v>-5</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="35">
         <f t="shared" si="0"/>
         <v>2.3423868312757219</v>
       </c>
-      <c r="I9" s="55"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="19">
         <f>SUM(B6:B9)</f>
         <v>0.99999999999999967</v>
@@ -1423,18 +1498,18 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="33">
         <v>2.3423868312757214</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="50"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="20">
         <f>SUMPRODUCT(C6:C9,$B$6:$B$9)</f>
         <v>3.0164609053497928</v>
@@ -1457,10 +1532,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="52"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="22">
         <v>2.3423868312757197</v>
       </c>
@@ -1490,11 +1565,12 @@
   <dimension ref="C5:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="11" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1577,18 +1653,18 @@
     </row>
     <row r="12" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="32">
         <f>ABS(MIN($G$6:$K$9))+$H$13</f>
         <v>15</v>
       </c>
@@ -1620,23 +1696,28 @@
       </c>
     </row>
     <row r="18" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="32">
+      <c r="G18" s="67">
+        <f>G20*($M$19+$H$14)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="33">
-        <v>0</v>
-      </c>
-      <c r="I18" s="33">
-        <v>0</v>
-      </c>
-      <c r="J18" s="33">
-        <v>0</v>
-      </c>
-      <c r="K18" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="68">
+        <f t="shared" ref="H18:K18" si="0">H20*($M$19+$H$14)</f>
+        <v>0.19039780521262017</v>
+      </c>
+      <c r="I18" s="68">
+        <f t="shared" si="0"/>
+        <v>0.19149519890260611</v>
+      </c>
+      <c r="J18" s="68">
+        <f t="shared" si="0"/>
+        <v>0.31522633744855977</v>
+      </c>
+      <c r="K18" s="69">
+        <f t="shared" si="0"/>
+        <v>0.30288065843621403</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G19" s="16" t="s">
         <v>19</v>
       </c>
@@ -1652,34 +1733,47 @@
       <c r="K19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="26"/>
+      <c r="M19" s="65">
+        <f>1/M25-H14</f>
+        <v>2.3423868312757214</v>
+      </c>
     </row>
     <row r="20" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="64" t="s">
+      <c r="G20" s="70">
+        <v>0</v>
+      </c>
+      <c r="H20" s="71">
+        <v>1.0978754370145389E-2</v>
+      </c>
+      <c r="I20" s="71">
+        <v>1.1042032493316235E-2</v>
+      </c>
+      <c r="J20" s="71">
+        <v>1.8176640880831478E-2</v>
+      </c>
+      <c r="K20" s="72">
+        <v>1.7464761995159225E-2</v>
+      </c>
+      <c r="L20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="55"/>
+      <c r="M20" s="43"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="61">
         <f>F21*($G$26+$H$14)</f>
         <v>0.49382716049382686</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="59">
         <v>2.8475155426890001E-2</v>
       </c>
       <c r="G21" s="6">
@@ -1687,200 +1781,200 @@
         <v>23</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" ref="H21:K21" si="0">H6+$H$14</f>
+        <f t="shared" ref="H21:K21" si="1">H6+$H$14</f>
         <v>10</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="K21" s="7">
-        <f t="shared" si="0"/>
+      <c r="K21" s="6">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="L21" s="60">
+      <c r="L21" s="45">
         <f>SUMPRODUCT($G$20:$K$20,G21:K21)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="61"/>
+        <v>1</v>
+      </c>
+      <c r="M21" s="46"/>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="38">
-        <f t="shared" ref="D22:D24" si="1">F22*($G$26+$H$14)</f>
+      <c r="D22" s="62">
+        <f t="shared" ref="D22:D24" si="2">F22*($G$26+$H$14)</f>
         <v>9.0534979423866815E-3</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="60">
         <v>5.2204451615964166E-4</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" ref="G22:K22" si="2">G7+$H$14</f>
+        <f t="shared" ref="G22:K22" si="3">G7+$H$14</f>
         <v>3</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="K22" s="7">
-        <f t="shared" si="2"/>
+      <c r="K22" s="6">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="L22" s="62">
-        <f t="shared" ref="L22:L24" si="3">SUMPRODUCT($G$20:$K$20,G22:K22)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="63"/>
+      <c r="L22" s="47">
+        <f t="shared" ref="L22:L24" si="4">SUMPRODUCT($G$20:$K$20,G22:K22)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="M22" s="48"/>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="38">
-        <f t="shared" si="1"/>
+      <c r="D23" s="62">
+        <f t="shared" si="2"/>
         <v>0.46337448559670835</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="60">
         <v>2.6719187508898498E-2</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" ref="G23:K23" si="4">G8+$H$14</f>
+        <f t="shared" ref="G23:K23" si="5">G8+$H$14</f>
         <v>13</v>
       </c>
       <c r="H23" s="6">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="L23" s="47">
         <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="I23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="48"/>
+    </row>
+    <row r="24" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="63">
+        <f t="shared" si="2"/>
+        <v>3.3744855967078116E-2</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="60">
+        <v>1.9458022875041472E-3</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" ref="G24:K24" si="6">G9+$H$14</f>
+        <v>18</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="L24" s="49">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J23" s="6">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="K23" s="7">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="L23" s="62">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="63"/>
-    </row>
-    <row r="24" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="39">
-        <f t="shared" si="1"/>
-        <v>3.3744855967078116E-2</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="30">
-        <v>1.9458022875041472E-3</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" ref="G24:K24" si="5">G9+$H$14</f>
-        <v>18</v>
-      </c>
-      <c r="H24" s="6">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="I24" s="6">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="J24" s="6">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="K24" s="7">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="L24" s="62">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="63"/>
+        <v>1</v>
+      </c>
+      <c r="M24" s="50"/>
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="58"/>
-      <c r="G25" s="45">
+      <c r="F25" s="75"/>
+      <c r="G25" s="73">
         <f>SUMPRODUCT($F$21:$F$24,G21:G24)</f>
         <v>1.0388685871577041</v>
       </c>
-      <c r="H25" s="46">
-        <f t="shared" ref="H25:K25" si="6">SUMPRODUCT($F$21:$F$24,H21:H24)</f>
+      <c r="H25" s="51">
+        <f t="shared" ref="H25:K25" si="7">SUMPRODUCT($F$21:$F$24,H21:H24)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="I25" s="46">
-        <f t="shared" si="6"/>
+      <c r="I25" s="51">
+        <f t="shared" si="7"/>
         <v>0.99999999999999944</v>
       </c>
-      <c r="J25" s="46">
-        <f t="shared" si="6"/>
+      <c r="J25" s="51">
+        <f t="shared" si="7"/>
         <v>0.999999999999999</v>
       </c>
-      <c r="K25" s="47">
-        <f t="shared" si="6"/>
+      <c r="K25" s="52">
+        <f t="shared" si="7"/>
         <v>0.99999999999999922</v>
       </c>
-      <c r="L25" s="41" t="s">
+      <c r="L25" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="40">
+      <c r="M25" s="56">
         <f>SUM(G20:K20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="E26" s="53" t="s">
+        <v>5.7662189739452321E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="56"/>
-      <c r="G26" s="42">
+      <c r="F26" s="77"/>
+      <c r="G26" s="58">
         <f>1/G27-H14</f>
         <v>2.3423868312757321</v>
       </c>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="44"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="64"/>
     </row>
     <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="31">
+      <c r="F27" s="55"/>
+      <c r="G27" s="57">
         <f>SUM(F21:F24)</f>
         <v>5.7662189739452287E-2</v>
       </c>
@@ -1890,15 +1984,11 @@
       <c r="K27" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="4">
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>